<commit_message>
corrigiendo #43 escala colores
43
</commit_message>
<xml_diff>
--- a/data/parametros_variables.xlsx
+++ b/data/parametros_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\odes-unidades-shiny-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD426FDA-F29F-41AA-8567-79424C691949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE3D1FA-AB4B-4B2E-9890-6AF2A37F77E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>44</v>
@@ -721,7 +721,7 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
agregar variables zcsm_ y zcndvi_
</commit_message>
<xml_diff>
--- a/data/parametros_variables.xlsx
+++ b/data/parametros_variables.xlsx
@@ -304,7 +304,7 @@
     <t xml:space="preserve">Anomalía del NDVI acumulado a 12 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">zcsm-1</t>
+    <t xml:space="preserve">zcsm_1</t>
   </si>
   <si>
     <t xml:space="preserve">zcSM 1 mes</t>
@@ -313,7 +313,7 @@
     <t xml:space="preserve">Anomalía de humedad de suelo (1m) acumulada a 1 mes.</t>
   </si>
   <si>
-    <t xml:space="preserve">zcsm-3</t>
+    <t xml:space="preserve">zcsm_3</t>
   </si>
   <si>
     <t xml:space="preserve">zcSM 3 meses</t>
@@ -322,7 +322,7 @@
     <t xml:space="preserve">Anomalía de humedad de suelo (1m) acumulada a 3 meses.</t>
   </si>
   <si>
-    <t xml:space="preserve">zcsm-6</t>
+    <t xml:space="preserve">zcsm_6</t>
   </si>
   <si>
     <t xml:space="preserve">zcSM 6 meses</t>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">Anomalía de humedad de suelo (1m) acumulada a 6 meses.</t>
   </si>
   <si>
-    <t xml:space="preserve">zcsm-12</t>
+    <t xml:space="preserve">zcsm_12</t>
   </si>
   <si>
     <t xml:space="preserve">zcSM 12 meses</t>
@@ -340,7 +340,7 @@
     <t xml:space="preserve">Anomalía de humedad de suelo (1m) acumulada a 12 meses.</t>
   </si>
   <si>
-    <t xml:space="preserve">zcsm-24</t>
+    <t xml:space="preserve">zcsm_24</t>
   </si>
   <si>
     <t xml:space="preserve">zcSM 24 meses</t>
@@ -349,7 +349,7 @@
     <t xml:space="preserve">Anomalía de humedad de suelo (1m) acumulada a 24 meses.</t>
   </si>
   <si>
-    <t xml:space="preserve">zcsm-36</t>
+    <t xml:space="preserve">zcsm_36</t>
   </si>
   <si>
     <t xml:space="preserve">zcSM 36 meses</t>
@@ -370,6 +370,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -564,10 +565,10 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="A25:E27"/>
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.41"/>

</xml_diff>

<commit_message>
arreglar reporte y planilla de parámetros
</commit_message>
<xml_diff>
--- a/data/parametros_variables.xlsx
+++ b/data/parametros_variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="121">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -118,6 +118,9 @@
     <t xml:space="preserve">SWEI</t>
   </si>
   <si>
+    <t xml:space="preserve">Índice estandarizado  de contenido de agua equivalente de nieve.</t>
+  </si>
+  <si>
     <t xml:space="preserve">spei_1</t>
   </si>
   <si>
@@ -127,7 +130,7 @@
     <t xml:space="preserve">#ff1820, #ff525e, #ff9ba1, #ffebed, #99dddf, #52bdc9, #127eaf</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía SPEI. Este índice indica la anomalía de la precipitación menos la evapotranspiración en 1 mes.</t>
+    <t xml:space="preserve">Anomalía de la precipitación menos la evapotranspiración acumulada en 1 mes.</t>
   </si>
   <si>
     <t xml:space="preserve">spei_3</t>
@@ -136,7 +139,23 @@
     <t xml:space="preserve">SPEI 3 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía SPEI. Este índice indica la anomalía de la precipitación menos la evapotranspiración en 3 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación menos la evapotranspiración acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 3 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spei_6</t>
@@ -145,7 +164,23 @@
     <t xml:space="preserve">SPEI 6 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía SPEI. Este índice indica la anomalía de la precipitación menos la evapotranspiración en 6 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación menos la evapotranspiración acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 6 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spei_12</t>
@@ -154,7 +189,23 @@
     <t xml:space="preserve">SPEI 12 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía SPEI. Este índice indica la anomalía de la precipitación menos la evapotranspiración en 12 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación menos la evapotranspiración acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 12 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spei_24</t>
@@ -163,7 +214,23 @@
     <t xml:space="preserve">SPEI 24 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía SPEI. Este índice indica la anomalía de la precipitación menos la evapotranspiración en 24 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación menos la evapotranspiración acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 24 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spei_36</t>
@@ -172,7 +239,23 @@
     <t xml:space="preserve">SPEI 36 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía SPEI. Este índice indica la anomalía de la precipitación menos la evapotranspiración en 36 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación menos la evapotranspiración acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 36 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spi_1</t>
@@ -184,7 +267,23 @@
     <t xml:space="preserve">#730000, #e60000, #ffaa00, #fcd37f, #ffff00</t>
   </si>
   <si>
-    <t xml:space="preserve">Indice de sequía SPI. Este índice indica la anomalía de la precipitación acumulada en 1 mes.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 1 mes.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spi_3</t>
@@ -193,7 +292,23 @@
     <t xml:space="preserve">SPI 3 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Indice de sequía SPI. Este índice indica la anomalía de la precipitación acumulada en 3 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 3 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spi_6</t>
@@ -202,7 +317,23 @@
     <t xml:space="preserve">SPI 6 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Indice de sequía SPI. Este índice indica la anomalía de la precipitación acumulada en 6 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación acumulada en en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 6 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spi_12</t>
@@ -211,7 +342,23 @@
     <t xml:space="preserve">SPI 12 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Indice de sequía SPI. Este índice indica la anomalía de la precipitación acumulada en 12 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> en 12 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spi_24</t>
@@ -220,7 +367,23 @@
     <t xml:space="preserve">SPI 24 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Indice de sequía SPI. Este índice indica la anomalía de la precipitación acumulada en 24 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> en 24 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">spi_36</t>
@@ -229,7 +392,23 @@
     <t xml:space="preserve">SPI 36 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Indice de sequía SPI. Este índice indica la anomalía de la precipitación acumulada en 36 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la precipitación acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> en 36 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eddi_1</t>
@@ -241,7 +420,7 @@
     <t xml:space="preserve">#127eaf, #52bdc9, #99dddf, #ffebed, #ff9ba1, #ff525e, #ff1820</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía de Demana evaporativa acumulado en 1 mes.</t>
+    <t xml:space="preserve">Anomalía de la demanda evaporativa de la atmosfera acumulada en 1 mes.</t>
   </si>
   <si>
     <t xml:space="preserve">eddi_3</t>
@@ -250,7 +429,23 @@
     <t xml:space="preserve">EDDI 3 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía de Demana evaporativa acumulado en 3 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la demanda evaporativa de la atmosfera acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 3 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eddi_6</t>
@@ -259,7 +454,23 @@
     <t xml:space="preserve">EDDI 6 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía de Demana evaporativa acumulado en 6 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la demanda evaporativa de la atmosfera acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 6 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eddi_12</t>
@@ -268,7 +479,23 @@
     <t xml:space="preserve">EDDI 12 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía de Demana evaporativa acumulado en 12 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la demanda evaporativa de la atmosfera acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 12 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eddi_24</t>
@@ -277,7 +504,23 @@
     <t xml:space="preserve">EDDI 24 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía de Demana evaporativa acumulado en 24 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la demanda evaporativa de la atmosfera acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 24 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eddi_36</t>
@@ -286,7 +529,23 @@
     <t xml:space="preserve">EDDI 36 meses</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de sequía de Demana evaporativa acumulado en 36 meses.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Anomalía de la demanda evaporativa de la atmosfera acumulada en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 36 meses.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">zcndvi_1</t>
@@ -389,7 +648,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -432,6 +691,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -487,7 +751,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -505,6 +769,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,11 +856,11 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.41"/>
@@ -738,6 +1006,9 @@
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -747,371 +1018,374 @@
         <v>31</v>
       </c>
       <c r="D9" s="3"/>
+      <c r="E9" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>47</v>
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="0" t="s">
         <v>54</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>63</v>
+        <v>54</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>69</v>
+        <v>54</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>85</v>
+        <v>73</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>88</v>
+        <v>73</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="D31" s="5"/>
       <c r="E31" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>